<commit_message>
update mrip figures in indicator table
</commit_message>
<xml_diff>
--- a/docs/bsb_indicator_table.xlsx
+++ b/docs/bsb_indicator_table.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nefscdata\SOE_ESP_Data\bsb\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stephanie.owen\Documents\bsb\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07733B7-4C89-4BFA-8D9C-1175ADA8E52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3825" windowWidth="29040" windowHeight="15720" xr2:uid="{F94664DC-F3F8-4BF8-B91D-6BF15F2C8F86}"/>
+    <workbookView xWindow="-28920" yWindow="-3828" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -105,12 +104,6 @@
     <t>swv_facet.png</t>
   </si>
   <si>
-    <t>total_recreational_trips_n_millions_2025-02-18.png</t>
-  </si>
-  <si>
-    <t>total_recreational_landings_lbs_millions_2025-02-18.png</t>
-  </si>
-  <si>
     <t>AVGVESREVperYr_BLACK_SEABASS_2023_DOLlb_2025-02-18.png</t>
   </si>
   <si>
@@ -142,12 +135,18 @@
   </si>
   <si>
     <t>Commercial revenue per vessel (2024 USD)</t>
+  </si>
+  <si>
+    <t>total_recreational_trips_n_millions_2025-04-03.png</t>
+  </si>
+  <si>
+    <t>total_recreational_landings_lbs_millions_2025-04-03.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -549,21 +548,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{616C184B-97FE-4AFC-A455-4B1A01E2E914}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="51.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="51.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -577,21 +576,21 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -603,7 +602,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="93" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -623,18 +622,18 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="115.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -643,18 +642,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -663,18 +662,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -683,18 +682,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E7">
         <v>3</v>

</xml_diff>

<commit_message>
remove text about preliminary 2024 mrip data
</commit_message>
<xml_diff>
--- a/docs/bsb_indicator_table.xlsx
+++ b/docs/bsb_indicator_table.xlsx
@@ -80,15 +80,9 @@
     <t>MRIP recreational trips (millions of annual trips)</t>
   </si>
   <si>
-    <t>Recent trip numbers are near an all-time high, but may have decreased from 2023 (2024 data is preliminary and does not include November and December 2024). Catch (not shown) generally reflects trip patterns. High regulatory complexity is likely contributing to recreational fishing trends.</t>
-  </si>
-  <si>
     <t>MRIP recreational landings (millions of lbs.)</t>
   </si>
   <si>
-    <t>The recreational black sea bass fishery has a catch-and-release component, and management measures are being implemented to reduce recreational harvest. 2024 data is preliminary and does not include November and December 2024.</t>
-  </si>
-  <si>
     <t>Number of commercial vessels (#)</t>
   </si>
   <si>
@@ -141,6 +135,12 @@
   </si>
   <si>
     <t>total_recreational_landings_lbs_millions_2025-04-03.png</t>
+  </si>
+  <si>
+    <t>Recent trip numbers are near an all-time high, but have decreased from 2023. Catch (not shown) generally reflects trip patterns. High regulatory complexity is likely contributing to recreational fishing trends.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The recreational black sea bass fishery has a catch-and-release component, and management measures are being implemented to reduce recreational harvest. </t>
   </si>
 </sst>
 </file>
@@ -552,7 +552,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,10 +576,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -587,13 +587,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="3" spans="1:6" ht="93" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -613,7 +613,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -622,18 +622,18 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -642,18 +642,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -664,16 +664,16 @@
     </row>
     <row r="6" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -684,16 +684,16 @@
     </row>
     <row r="7" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <v>3</v>

</xml_diff>

<commit_message>
update bsb commercial indicators
</commit_message>
<xml_diff>
--- a/docs/bsb_indicator_table.xlsx
+++ b/docs/bsb_indicator_table.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stephanie.owen\Documents\bsb\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nefscdata\SOE_ESP_Data\bsb\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16352D6-958B-447E-B994-DC5475C71C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3828" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,15 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -98,12 +90,6 @@
     <t>swv_facet.png</t>
   </si>
   <si>
-    <t>AVGVESREVperYr_BLACK_SEABASS_2023_DOLlb_2025-02-18.png</t>
-  </si>
-  <si>
-    <t>N_Commercial_Vessels_Landing_BLACK_SEABASS_2025-02-18.png</t>
-  </si>
-  <si>
     <t>North: Below threshold South: Near long-term average</t>
   </si>
   <si>
@@ -141,13 +127,19 @@
   </si>
   <si>
     <t xml:space="preserve">The recreational black sea bass fishery has a catch-and-release component, and management measures are being implemented to reduce recreational harvest. </t>
+  </si>
+  <si>
+    <t>N_Commercial_Vessels_Landing_BLACK_SEABASS_2025-04-17.png</t>
+  </si>
+  <si>
+    <t>AVGVESREVperYr_BLACK_SEABASS_2024_DOLlb_2025-04-17.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +166,11 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -223,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -234,6 +231,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -548,21 +548,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
-    <col min="3" max="3" width="51.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="51.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="61.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -576,21 +577,21 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -602,7 +603,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="93" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="90" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -622,18 +623,18 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -642,18 +643,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -662,18 +663,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -682,18 +683,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E7">
         <v>3</v>

</xml_diff>